<commit_message>
fix execute code func: test_case with "; " was handled incorrectly
</commit_message>
<xml_diff>
--- a/data/test/merged_executed.xlsx
+++ b/data/test/merged_executed.xlsx
@@ -583,7 +583,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>ValueError("could not convert string to float: '0.1; 500'")</t>
+          <t>Реализация проекта будет стоить {money} тыс. руб. без скидки. Со скидой стоимость составит {money- (money * discount)} тыс. руб.</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -665,7 +665,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>SyntaxError('unterminated string literal (detected at line 6)', ('&lt;string&gt;', 6, 7, "print(f'Реализация проекта будет стоить {money} тыс. руб. без скидки. Со скидой стоимость составит {money- (money * discount)} тыс. руб.)", 6, 7))</t>
+          <t>SyntaxError('unterminated f-string literal (detected at line 6)', ('&lt;string&gt;', 6, 7, "print(f'Реализация проекта будет стоить {money} тыс. руб. без скидки. Со скидой стоимость составит {money- (money * discount)} тыс. руб.)", 6, 7))</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>ValueError("could not convert string to float: '0.1; 500'")</t>
+          <t>Реализация проекта будет стоить 0.1 тыс. руб. без скидки. Со скидой стоимость составит 450.0 тыс. руб.</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -911,7 +911,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>ValueError("could not convert string to float: '0.1; 500'")</t>
+          <t>Реализация проекта будет стоить 500 тыс. руб. без скидки. Со скидой стоимость составит 50.0 тыс. руб.</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -993,7 +993,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>SyntaxError('unterminated string literal (detected at line 6)', ('&lt;string&gt;', 6, 7, 'print(f"Реализация проекта будет стоить {money} тыс. руб. без скидки. Со скидой стоимость составит {money- (money * discount)} тыс. руб.\')', 6, 7))</t>
+          <t>SyntaxError('unterminated f-string literal (detected at line 6)', ('&lt;string&gt;', 6, 7, 'print(f"Реализация проекта будет стоить {money} тыс. руб. без скидки. Со скидой стоимость составит {money- (money * discount)} тыс. руб.\')', 6, 7))</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1075,12 +1075,12 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>ValueError("could not convert string to float: '0.1; 500'")</t>
+          <t>Реализация проекта будет стоить 500 тыс. руб. без скидки. Со скидкой стоимость составит 450.0 тыс. руб.</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>ValueError("could not convert string to float: '0.1; 500'")</t>
+          <t>Реализация проекта будет стоить money тыс. руб. без скидки. Со скидой стоимость составит money- (money * discount) тыс. руб.</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>{'Пурпурный', 'Серый', 'Желтый'}</t>
+          <t>{'Серый', 'Пурпурный', 'Желтый'}</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Пурпурный; Серый; Желтый</t>
+          <t>Серый; Пурпурный; Желтый</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -4251,7 +4251,7 @@
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 6, 25, '        if room not in v\n', 6, 25))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 6, 25, '        if room not in v\n', 6, 26))</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -4513,7 +4513,7 @@
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>SyntaxError('unterminated string literal (detected at line 6)', ('&lt;string&gt;', 6, 7, "print(f'Реализация проекта будет стоить {money} тыс. руб. Срок реализации проекта {duration} недель.)", 6, 7))</t>
+          <t>SyntaxError('unterminated f-string literal (detected at line 6)', ('&lt;string&gt;', 6, 7, "print(f'Реализация проекта будет стоить {money} тыс. руб. Срок реализации проекта {duration} недель.)", 6, 7))</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -5765,7 +5765,7 @@
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 6, 55, 'if color not in logo_project and color in cite_project\n', 6, 55))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 6, 55, 'if color not in logo_project and color in cite_project\n', 6, 56))</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -7751,7 +7751,7 @@
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>{'Патиново-зеленый', 'Оливковый', 'Пастельно-зеленый'}</t>
+          <t>{'Оливковый', 'Патиново-зеленый', 'Пастельно-зеленый'}</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -7837,7 +7837,7 @@
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Патиново-зеленый Оливковый Пастельно-зеленый</t>
+          <t>Оливковый Патиново-зеленый Пастельно-зеленый</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -9278,7 +9278,7 @@
       </c>
       <c r="O101" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 6, 22, '        if room  in v\n', 6, 22))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 6, 22, '        if room  in v\n', 6, 23))</t>
         </is>
       </c>
       <c r="P101" t="inlineStr">
@@ -10833,7 +10833,7 @@
       </c>
       <c r="O117" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 4, 24, '    for line in my_file\n', 4, 24))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 4, 24, '    for line in my_file\n', 4, 25))</t>
         </is>
       </c>
       <c r="P117" t="inlineStr">
@@ -12654,7 +12654,7 @@
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 9, 16, 'for item in res\n', 9, 16))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 9, 16, 'for item in res\n', 9, 17))</t>
         </is>
       </c>
       <c r="P137" t="inlineStr">
@@ -13068,11 +13068,7 @@
         <is>
           <t>3000
 28000
-28000
-90000
-90000
-150000
-150000</t>
+28000</t>
         </is>
       </c>
       <c r="P141" t="inlineStr">
@@ -13380,12 +13376,12 @@
       </c>
       <c r="O144" t="inlineStr">
         <is>
-          <t>90000</t>
+          <t>28000</t>
         </is>
       </c>
       <c r="P144" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -13787,7 +13783,7 @@
       </c>
       <c r="O148" t="inlineStr">
         <is>
-          <t>10000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="P148" t="inlineStr">
@@ -13890,7 +13886,7 @@
       </c>
       <c r="O149" t="inlineStr">
         <is>
-          <t>10000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="P149" t="inlineStr">
@@ -13999,7 +13995,7 @@
       </c>
       <c r="O150" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 1, 15, 'def work(slov)\n', 1, 15))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 1, 15, 'def work(slov)\n', 1, 16))</t>
         </is>
       </c>
       <c r="P150" t="inlineStr">
@@ -15949,7 +15945,7 @@
       </c>
       <c r="O169" t="inlineStr">
         <is>
-          <t>SyntaxError('unterminated string literal (detected at line 5)', ('&lt;string&gt;', 5, 7, 'print(f"Сегодня мы будем анализировать {ton} в тексте!)', 5, 7))</t>
+          <t>SyntaxError('unterminated f-string literal (detected at line 5)', ('&lt;string&gt;', 5, 7, 'print(f"Сегодня мы будем анализировать {ton} в тексте!)', 5, 7))</t>
         </is>
       </c>
       <c r="P169" t="inlineStr">
@@ -16941,7 +16937,7 @@
       </c>
       <c r="O181" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 7, 75, "if language.endswith('есть') and language.split('-')[1] == second_language\n", 7, 75))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 7, 75, "if language.endswith('есть') and language.split('-')[1] == second_language\n", 7, 76))</t>
         </is>
       </c>
       <c r="P181" t="inlineStr">
@@ -20225,7 +20221,7 @@
       </c>
       <c r="O217" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 8, 23, '    if skill in skills\n', 8, 23))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 8, 23, '    if skill in skills\n', 8, 24))</t>
         </is>
       </c>
       <c r="P217" t="inlineStr">
@@ -21511,7 +21507,7 @@
       </c>
       <c r="O230" t="inlineStr">
         <is>
-          <t>SyntaxError('unterminated string literal (detected at line 5)', ('&lt;string&gt;', 5, 7, "print(f'В агентстве «Шедеврус» мы делаем дизайн за {time}!)", 5, 7))</t>
+          <t>SyntaxError('unterminated f-string literal (detected at line 5)', ('&lt;string&gt;', 5, 7, "print(f'В агентстве «Шедеврус» мы делаем дизайн за {time}!)", 5, 7))</t>
         </is>
       </c>
       <c r="P230" t="inlineStr">
@@ -22064,7 +22060,7 @@
       </c>
       <c r="O237" t="inlineStr">
         <is>
-          <t>SyntaxError('unterminated string literal (detected at line 5)', ('&lt;string&gt;', 5, 7, 'print(f"В агентстве «Шедеврус» мы делаем дизайн за {time}!\')', 5, 7))</t>
+          <t>SyntaxError('unterminated f-string literal (detected at line 5)', ('&lt;string&gt;', 5, 7, 'print(f"В агентстве «Шедеврус» мы делаем дизайн за {time}!\')', 5, 7))</t>
         </is>
       </c>
       <c r="P237" t="inlineStr">
@@ -23154,7 +23150,7 @@
       </c>
       <c r="O249" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 11, 5, 'else\n', 11, 5))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 11, 5, 'else\n', 11, 6))</t>
         </is>
       </c>
       <c r="P249" t="inlineStr">
@@ -24083,7 +24079,7 @@
       </c>
       <c r="O259" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 5, 17, '    if font in v\n', 5, 17))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 5, 17, '    if font in v\n', 5, 18))</t>
         </is>
       </c>
       <c r="P259" t="inlineStr">
@@ -24455,7 +24451,7 @@
       </c>
       <c r="O263" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 1, 32, 'def best_agencies(names, count)\n', 1, 32))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 1, 32, 'def best_agencies(names, count)\n', 1, 33))</t>
         </is>
       </c>
       <c r="P263" t="inlineStr">
@@ -27661,11 +27657,7 @@
           <t>['Музей изобразительных искусств, Новая Третьяковка, Пушкинский музей', 'Московский музей современного искусства', nan]</t>
         </is>
       </c>
-      <c r="O297" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Музей изобразительных искусств,  Пушкинский музей, Новая Третьяковка</t>
-        </is>
-      </c>
+      <c r="O297" t="inlineStr"/>
       <c r="P297" t="inlineStr">
         <is>
           <t>0</t>
@@ -27973,7 +27965,7 @@
       <c r="O300" t="inlineStr"/>
       <c r="P300" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -28271,11 +28263,7 @@
           <t>['Музей изобразительных искусств, Новая Третьяковка, Пушкинский музей', 'Московский музей современного искусства', nan]</t>
         </is>
       </c>
-      <c r="O303" t="inlineStr">
-        <is>
-          <t>август, октябрь, декабрь, февраль, апрель, июнь, август, январь, март, май, август</t>
-        </is>
-      </c>
+      <c r="O303" t="inlineStr"/>
       <c r="P303" t="inlineStr">
         <is>
           <t>0</t>
@@ -28374,11 +28362,7 @@
           <t>['Музей изобразительных искусств, Новая Третьяковка, Пушкинский музей', 'Московский музей современного искусства', nan]</t>
         </is>
       </c>
-      <c r="O304" t="inlineStr">
-        <is>
-          <t>AttributeError("'list' object has no attribute 'add'")</t>
-        </is>
-      </c>
+      <c r="O304" t="inlineStr"/>
       <c r="P304" t="inlineStr">
         <is>
           <t>0</t>
@@ -28479,7 +28463,7 @@
       </c>
       <c r="O305" t="inlineStr">
         <is>
-          <t>Эрмитаж</t>
+          <t>Новая Третьяковка</t>
         </is>
       </c>
       <c r="P305" t="inlineStr">
@@ -28582,7 +28566,7 @@
       </c>
       <c r="O306" t="inlineStr">
         <is>
-          <t>['Новая Третьяковка', 'Пушкинский музей', 'Музей изобразительных искусств']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="P306" t="inlineStr">
@@ -28683,11 +28667,7 @@
           <t>['Музей изобразительных искусств, Новая Третьяковка, Пушкинский музей', 'Московский музей современного искусства', nan]</t>
         </is>
       </c>
-      <c r="O307" t="inlineStr">
-        <is>
-          <t>Музей изобразительных искусств Новая Третьяковка Пушкинский музей</t>
-        </is>
-      </c>
+      <c r="O307" t="inlineStr"/>
       <c r="P307" t="inlineStr">
         <is>
           <t>0</t>
@@ -28786,11 +28766,7 @@
           <t>['Музей изобразительных искусств, Новая Третьяковка, Пушкинский музей', 'Московский музей современного искусства', nan]</t>
         </is>
       </c>
-      <c r="O308" t="inlineStr">
-        <is>
-          <t>Пушкинский музей, Новая Третьяковка, Музей изобразительных искусств</t>
-        </is>
-      </c>
+      <c r="O308" t="inlineStr"/>
       <c r="P308" t="inlineStr">
         <is>
           <t>0</t>
@@ -28889,14 +28865,7 @@
           <t>['Музей изобразительных искусств, Новая Третьяковка, Пушкинский музей', 'Московский музей современного искусства', nan]</t>
         </is>
       </c>
-      <c r="O309" t="inlineStr">
-        <is>
-          <t>Новая Третьяковка
-Новая Третьяковка
-Новая Третьяковка, Пушкинский музей
-Музей изобразительных искусств, Новая Третьяковка, Пушкинский музей</t>
-        </is>
-      </c>
+      <c r="O309" t="inlineStr"/>
       <c r="P309" t="inlineStr">
         <is>
           <t>0</t>
@@ -28995,11 +28964,7 @@
           <t>['Музей изобразительных искусств, Новая Третьяковка, Пушкинский музей', 'Московский музей современного искусства', nan]</t>
         </is>
       </c>
-      <c r="O310" t="inlineStr">
-        <is>
-          <t>Музей изобразительных искусств,Новая Третьяковка,Пушкинский музей</t>
-        </is>
-      </c>
+      <c r="O310" t="inlineStr"/>
       <c r="P310" t="inlineStr">
         <is>
           <t>0</t>
@@ -29099,7 +29064,7 @@
       </c>
       <c r="O311" t="inlineStr">
         <is>
-          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 1, 18, 'def success(data)\n', 1, 18))</t>
+          <t>SyntaxError("expected ':'", ('&lt;string&gt;', 1, 18, 'def success(data)\n', 1, 19))</t>
         </is>
       </c>
       <c r="P311" t="inlineStr">

</xml_diff>